<commit_message>
very rename so sheets wow intensifies fix #5
</commit_message>
<xml_diff>
--- a/resources/test_array.xlsx
+++ b/resources/test_array.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="14580" yWindow="3220" windowWidth="25600" windowHeight="18380" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="test.json" sheetId="1" r:id="rId1"/>
-    <sheet name="test.json#properties" sheetId="3" r:id="rId2"/>
+    <sheet name="test_array.json" sheetId="1" r:id="rId1"/>
+    <sheet name="test_array.json#properties" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>

</xml_diff>